<commit_message>
Working on fixing the AC printout, not compiling
</commit_message>
<xml_diff>
--- a/20161127 todos.xlsx
+++ b/20161127 todos.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13065" windowHeight="5370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13065" windowHeight="5370" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Current" sheetId="1" r:id="rId1"/>
+    <sheet name="New Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$E$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Current!$A$5:$E$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Key for Quad chart</t>
   </si>
@@ -158,9 +159,6 @@
     <t>CV speech</t>
   </si>
   <si>
-    <t>AC on printout</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -252,6 +250,33 @@
   </si>
   <si>
     <t>L10 Todo Tile create todo for L10 not working</t>
+  </si>
+  <si>
+    <t>add AC on printout</t>
+  </si>
+  <si>
+    <t>Print button for VTO</t>
+  </si>
+  <si>
+    <t>Data Entry Slow on VTO</t>
+  </si>
+  <si>
+    <t>Bullet points for the 3yp</t>
+  </si>
+  <si>
+    <t>Multiple measurables in VTO</t>
+  </si>
+  <si>
+    <t>Monthly Scorecard metrics (bill undell)</t>
+  </si>
+  <si>
+    <t>Prioritize Todo list</t>
+  </si>
+  <si>
+    <t>VTO is hidden</t>
+  </si>
+  <si>
+    <t>Permissions for VTO</t>
   </si>
 </sst>
 </file>
@@ -640,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,33 +683,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H1" s="11">
-        <f>1-COUNTBLANK($A$6:A72)/ROWS($A$6:A72)</f>
-        <v>0.32835820895522383</v>
+        <f>1-COUNTBLANK($A$6:A73)/ROWS($A$6:A73)</f>
+        <v>0.32352941176470584</v>
       </c>
       <c r="I1" s="12">
         <f>H2/H3</f>
-        <v>0.32835820895522388</v>
+        <v>0.3235294117647059</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="3">
-        <f>ROWS($A$6:A72)-COUNTBLANK($A$6:A72)</f>
+        <f>ROWS($A$6:A73)-COUNTBLANK($A$6:A73)</f>
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="4">
-        <f>ROWS(A6:A72)</f>
-        <v>67</v>
+        <f>ROWS(A6:A73)</f>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -692,13 +717,13 @@
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>29</v>
@@ -754,7 +779,7 @@
         <v>66.932802122726045</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8"/>
       <c r="H8" s="6"/>
@@ -772,9 +797,9 @@
         <v>63.63961030678928</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="F9"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -790,12 +815,12 @@
         <v>62.217360921209121</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" s="2">
         <v>70</v>
@@ -810,7 +835,7 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="F11"/>
+      <c r="F11" s="2"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -843,7 +868,7 @@
         <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13"/>
       <c r="H13" s="6"/>
@@ -851,53 +876,54 @@
     <row r="14" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2">
         <v>5</v>
       </c>
       <c r="D14" s="8">
         <f>SQRT(B14)*(C14)*IF(ISBLANK(A14),1,-1)</f>
-        <v>44.158804331639239</v>
+        <v>44.721359549995796</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="F14"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15"/>
       <c r="B15" s="2">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2">
         <v>5</v>
       </c>
       <c r="D15" s="8">
         <f>SQRT(B15)*(C15)*IF(ISBLANK(A15),1,-1)</f>
-        <v>43.301270189221938</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
+        <v>44.158804331639239</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
       </c>
       <c r="F15"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="8">
         <f>SQRT(B16)*(C16)*IF(ISBLANK(A16),1,-1)</f>
-        <v>42.426406871192853</v>
+        <v>43.301270189221938</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="F16"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -912,25 +938,24 @@
         <v>42.426406871192853</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17"/>
+        <v>32</v>
+      </c>
+      <c r="F17" s="2"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
       <c r="B18" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2">
         <v>6</v>
       </c>
       <c r="D18" s="8">
         <f>SQRT(B18)*(C18)*IF(ISBLANK(A18),1,-1)</f>
-        <v>40.693979898751607</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
+        <v>42.426406871192853</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F18"/>
       <c r="H18" s="6"/>
@@ -938,19 +963,19 @@
     <row r="19" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19" s="2">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19" s="8">
         <f>SQRT(B19)*(C19)*IF(ISBLANK(A19),1,-1)</f>
-        <v>40.311288741492746</v>
+        <v>40.693979898751607</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="F19"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -966,117 +991,120 @@
         <v>40.311288741492746</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
       <c r="B21" s="2">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" s="8">
         <f>SQRT(B21)*(C21)*IF(ISBLANK(A21),1,-1)</f>
-        <v>38.340579025361627</v>
+        <v>40.311288741492746</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="F21"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22" s="8">
         <f>SQRT(B22)*(C22)*IF(ISBLANK(A22),1,-1)</f>
-        <v>37.947331922020552</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>38.340579025361627</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
       <c r="B23" s="2">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" s="8">
         <f>SQRT(B23)*(C23)*IF(ISBLANK(A23),1,-1)</f>
-        <v>37.080992435478315</v>
-      </c>
-      <c r="E23" t="s">
-        <v>2</v>
-      </c>
+        <v>37.947331922020552</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" s="8">
         <f>SQRT(B24)*(C24)*IF(ISBLANK(A24),1,-1)</f>
-        <v>35.552777669262355</v>
+        <v>37.080992435478315</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C25" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="8">
         <f>SQRT(B25)*(C25)*IF(ISBLANK(A25),1,-1)</f>
-        <v>33.541019662496851</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>35.552777669262355</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D26" s="8">
         <f>SQRT(B26)*(C26)*IF(ISBLANK(A26),1,-1)</f>
-        <v>30.740852297878796</v>
-      </c>
-      <c r="E26" t="s">
-        <v>13</v>
-      </c>
+        <v>33.541019662496851</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27" s="8">
         <f>SQRT(B27)*(C27)*IF(ISBLANK(A27),1,-1)</f>
-        <v>30.724582991474431</v>
+        <v>30.740852297878796</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1091,72 +1119,72 @@
         <v>30.724582991474431</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
       <c r="B29" s="2">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="8">
         <f>SQRT(B29)*(C29)*IF(ISBLANK(A29),1,-1)</f>
-        <v>30.14962686336267</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>33</v>
+        <v>30.724582991474431</v>
+      </c>
+      <c r="E29" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C30" s="2">
         <v>3</v>
       </c>
       <c r="D30" s="8">
         <f>SQRT(B30)*(C30)*IF(ISBLANK(A30),1,-1)</f>
-        <v>30</v>
+        <v>30.14962686336267</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="2"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
       <c r="B31" s="2">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D31" s="8">
         <f>SQRT(B31)*(C31)*IF(ISBLANK(A31),1,-1)</f>
         <v>30</v>
       </c>
-      <c r="E31" t="s">
-        <v>20</v>
+      <c r="E31" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C32" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D32" s="8">
         <f>SQRT(B32)*(C32)*IF(ISBLANK(A32),1,-1)</f>
-        <v>26.832815729997478</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
@@ -1170,161 +1198,165 @@
         <v>26.832815729997478</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
       <c r="B34" s="2">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C34" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" s="8">
         <f>SQRT(B34)*(C34)*IF(ISBLANK(A34),1,-1)</f>
-        <v>25.98076211353316</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>42</v>
+        <v>26.832815729997478</v>
+      </c>
+      <c r="E34" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C35" s="2">
         <v>3</v>
       </c>
       <c r="D35" s="8">
         <f>SQRT(B35)*(C35)*IF(ISBLANK(A35),1,-1)</f>
-        <v>24.919871588754226</v>
+        <v>25.98076211353316</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="2"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
       <c r="B36" s="2">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C36" s="2">
         <v>3</v>
       </c>
       <c r="D36" s="8">
         <f>SQRT(B36)*(C36)*IF(ISBLANK(A36),1,-1)</f>
-        <v>24.556058315617349</v>
-      </c>
-      <c r="E36" t="s">
-        <v>60</v>
-      </c>
+        <v>24.919871588754226</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C37" s="2">
         <v>3</v>
       </c>
       <c r="D37" s="8">
         <f>SQRT(B37)*(C37)*IF(ISBLANK(A37),1,-1)</f>
-        <v>24.186773244895647</v>
+        <v>24.556058315617349</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="2"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C38" s="2">
         <v>3</v>
       </c>
       <c r="D38" s="8">
         <f>SQRT(B38)*(C38)*IF(ISBLANK(A38),1,-1)</f>
-        <v>23.237900077244504</v>
-      </c>
-      <c r="E38" s="2" t="s">
+        <v>24.186773244895647</v>
+      </c>
+      <c r="E38" t="s">
         <v>52</v>
       </c>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C39" s="2">
         <v>3</v>
       </c>
       <c r="D39" s="8">
         <f>SQRT(B39)*(C39)*IF(ISBLANK(A39),1,-1)</f>
-        <v>17.748239349298849</v>
-      </c>
-      <c r="E39" t="s">
-        <v>54</v>
-      </c>
+        <v>23.237900077244504</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
       <c r="B40" s="2">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C40" s="2">
         <v>3</v>
       </c>
       <c r="D40" s="8">
         <f>SQRT(B40)*(C40)*IF(ISBLANK(A40),1,-1)</f>
-        <v>16.431676725154983</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F40" s="2"/>
+        <v>17.748239349298849</v>
+      </c>
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>40</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
+      <c r="A41" s="1"/>
+      <c r="B41" s="2">
+        <v>30</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3</v>
       </c>
       <c r="D41" s="8">
         <f>SQRT(B41)*(C41)*IF(ISBLANK(A41),1,-1)</f>
-        <v>12.649110640673518</v>
-      </c>
-      <c r="E41" t="s">
-        <v>62</v>
-      </c>
+        <v>16.431676725154983</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2">
-        <v>25</v>
-      </c>
-      <c r="C42" s="2">
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" s="8">
         <f>SQRT(B42)*(C42)*IF(ISBLANK(A42),1,-1)</f>
-        <v>10</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>39</v>
+        <v>12.649110640673518</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="2">
+        <v>25</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
       <c r="D43" s="8">
         <f>SQRT(B43)*(C43)*IF(ISBLANK(A43),1,-1)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1334,8 +1366,8 @@
         <f>SQRT(B44)*(C44)*IF(ISBLANK(A44),1,-1)</f>
         <v>0</v>
       </c>
-      <c r="E44" t="s">
-        <v>16</v>
+      <c r="E44" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1346,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1368,9 +1400,8 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" s="2"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
@@ -1380,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -1392,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -1404,27 +1435,21 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
-        <v>42701</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
       <c r="D51" s="8">
         <f>SQRT(B51)*(C51)*IF(ISBLANK(A51),1,-1)</f>
-        <v>-1</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
@@ -1441,12 +1466,12 @@
         <v>-1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
-        <v>42697</v>
+        <v>42701</v>
       </c>
       <c r="B53" s="2">
         <v>1</v>
@@ -1459,12 +1484,12 @@
         <v>-1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
-        <v>42696</v>
+        <v>42697</v>
       </c>
       <c r="B54" s="2">
         <v>1</v>
@@ -1476,13 +1501,13 @@
         <f>SQRT(B54)*(C54)*IF(ISBLANK(A54),1,-1)</f>
         <v>-1</v>
       </c>
-      <c r="E54" t="s">
-        <v>8</v>
+      <c r="E54" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
-        <v>42681</v>
+        <v>42696</v>
       </c>
       <c r="B55" s="2">
         <v>1</v>
@@ -1495,13 +1520,12 @@
         <v>-1</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
-      </c>
-      <c r="F55" s="2"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
-        <v>42696</v>
+        <v>42681</v>
       </c>
       <c r="B56" s="2">
         <v>1</v>
@@ -1514,12 +1538,13 @@
         <v>-1</v>
       </c>
       <c r="E56" t="s">
-        <v>25</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
-        <v>42688</v>
+        <v>42696</v>
       </c>
       <c r="B57" s="2">
         <v>1</v>
@@ -1532,97 +1557,97 @@
         <v>-1</v>
       </c>
       <c r="E57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="10">
-        <v>42706</v>
+      <c r="A58" s="9">
+        <v>42688</v>
       </c>
       <c r="B58" s="2">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C58" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="8">
         <f>SQRT(B58)*(C58)*IF(ISBLANK(A58),1,-1)</f>
-        <v>-15.491933384829668</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>37</v>
+        <v>-1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+      <c r="A59" s="10">
         <v>42706</v>
       </c>
       <c r="B59" s="2">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C59" s="2">
         <v>2</v>
       </c>
       <c r="D59" s="8">
         <f>SQRT(B59)*(C59)*IF(ISBLANK(A59),1,-1)</f>
-        <v>-17.320508075688775</v>
-      </c>
-      <c r="E59" t="s">
-        <v>26</v>
+        <v>-15.491933384829668</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="10">
-        <v>42709</v>
+      <c r="A60" s="5">
+        <v>42706</v>
       </c>
       <c r="B60" s="2">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C60" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D60" s="8">
         <f>SQRT(B60)*(C60)*IF(ISBLANK(A60),1,-1)</f>
-        <v>-35.355339059327378</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>69</v>
+        <v>-17.320508075688775</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>42706</v>
+      <c r="A61" s="10">
+        <v>42709</v>
       </c>
       <c r="B61" s="2">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C61" s="2">
         <v>5</v>
       </c>
       <c r="D61" s="8">
         <f>SQRT(B61)*(C61)*IF(ISBLANK(A61),1,-1)</f>
-        <v>-42.720018726587654</v>
-      </c>
-      <c r="E61" t="s">
-        <v>6</v>
+        <v>-35.355339059327378</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="10">
+      <c r="A62" s="5">
         <v>42706</v>
       </c>
       <c r="B62" s="2">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C62" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62" s="8">
         <f>SQRT(B62)*(C62)*IF(ISBLANK(A62),1,-1)</f>
-        <v>-44.497190922573978</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>38</v>
+        <v>-42.720018726587654</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1630,191 +1655,209 @@
         <v>42706</v>
       </c>
       <c r="B63" s="2">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C63" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" s="8">
         <f>SQRT(B63)*(C63)*IF(ISBLANK(A63),1,-1)</f>
-        <v>-54.772255750516614</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>68</v>
+        <v>-44.497190922573978</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
-        <v>42709</v>
+      <c r="A64" s="10">
+        <v>42706</v>
       </c>
       <c r="B64" s="2">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C64" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D64" s="8">
         <f>SQRT(B64)*(C64)*IF(ISBLANK(A64),1,-1)</f>
-        <v>-60</v>
-      </c>
-      <c r="E64" t="s">
-        <v>73</v>
+        <v>-54.772255750516614</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>42705</v>
+        <v>42709</v>
       </c>
       <c r="B65" s="2">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C65" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D65" s="8">
         <f>SQRT(B65)*(C65)*IF(ISBLANK(A65),1,-1)</f>
-        <v>-66.775744099186198</v>
+        <v>-60</v>
       </c>
       <c r="E65" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="10">
-        <v>42706</v>
+      <c r="A66" s="5">
+        <v>42705</v>
       </c>
       <c r="B66" s="2">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C66" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="8">
         <f>SQRT(B66)*(C66)*IF(ISBLANK(A66),1,-1)</f>
-        <v>-66.932802122726045</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>35</v>
+        <v>-66.775744099186198</v>
+      </c>
+      <c r="E66" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
-        <v>42705</v>
+        <v>42706</v>
       </c>
       <c r="B67" s="2">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="C67" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D67" s="8">
         <f>SQRT(B67)*(C67)*IF(ISBLANK(A67),1,-1)</f>
-        <v>-70.710678118654755</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>71</v>
+        <v>-66.932802122726045</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="A68" s="10">
         <v>42705</v>
       </c>
       <c r="B68" s="2">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="C68" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D68" s="8">
         <f>SQRT(B68)*(C68)*IF(ISBLANK(A68),1,-1)</f>
-        <v>-71.105555338524709</v>
+        <v>-70.710678118654755</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
+      <c r="A69" s="9">
         <v>42705</v>
       </c>
       <c r="B69" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" s="2">
         <v>8</v>
       </c>
       <c r="D69" s="8">
         <f>SQRT(B69)*(C69)*IF(ISBLANK(A69),1,-1)</f>
-        <v>-71.554175279993274</v>
+        <v>-71.105555338524709</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
-        <v>42706</v>
+        <v>42705</v>
       </c>
       <c r="B70" s="2">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C70" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D70" s="8">
         <f>SQRT(B70)*(C70)*IF(ISBLANK(A70),1,-1)</f>
-        <v>-73.416619371910613</v>
-      </c>
-      <c r="E70" t="s">
-        <v>19</v>
+        <v>-71.554175279993274</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
-        <v>42701</v>
+        <v>42706</v>
       </c>
       <c r="B71" s="2">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C71" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D71" s="8">
         <f>SQRT(B71)*(C71)*IF(ISBLANK(A71),1,-1)</f>
-        <v>-89.095454429504983</v>
+        <v>-73.416619371910613</v>
       </c>
       <c r="E71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>42701</v>
+      </c>
+      <c r="B72" s="2">
+        <v>98</v>
+      </c>
+      <c r="C72" s="2">
         <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
-        <v>42703</v>
-      </c>
-      <c r="B72" s="2">
-        <v>100</v>
-      </c>
-      <c r="C72" s="2">
-        <v>10</v>
       </c>
       <c r="D72" s="8">
         <f>SQRT(B72)*(C72)*IF(ISBLANK(A72),1,-1)</f>
+        <v>-89.095454429504983</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
+        <v>42703</v>
+      </c>
+      <c r="B73" s="2">
+        <v>100</v>
+      </c>
+      <c r="C73" s="2">
+        <v>10</v>
+      </c>
+      <c r="D73" s="8">
+        <f>SQRT(B73)*(C73)*IF(ISBLANK(A73),1,-1)</f>
         <v>-100</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>64</v>
+      <c r="E73" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A5:E5">
-    <sortState ref="A6:E72">
+    <sortState ref="A6:E73">
       <sortCondition descending="1" ref="D5"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:E63">
     <sortCondition descending="1" ref="D2:D63"/>
   </sortState>
-  <conditionalFormatting sqref="H9:H20 H1">
+  <conditionalFormatting sqref="H10:H21 H1">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.9"/>
@@ -1829,4 +1872,54 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added key to Quad Chart. Fixed review printout overflow
</commit_message>
<xml_diff>
--- a/20161127 todos.xlsx
+++ b/20161127 todos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\RadialReview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\repos\Radial\RadialReview\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13065" windowHeight="5370" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11385" windowHeight="5370"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t xml:space="preserve">advanced settings not saving </t>
   </si>
   <si>
-    <t>Edit page error Rose</t>
-  </si>
-  <si>
     <t>Edit todos on conclusion</t>
   </si>
   <si>
@@ -195,18 +192,12 @@
     <t>Scorecard: * If only one attendee, set default to defaulttodo owner</t>
   </si>
   <si>
-    <t>Scorecard: * Receipts</t>
-  </si>
-  <si>
     <t>Auto gen Team :* Auto delete</t>
   </si>
   <si>
     <t>Auto gen Team :* Auto fix name</t>
   </si>
   <si>
-    <t>Jennifers teams:* Blinker</t>
-  </si>
-  <si>
     <t>When issue moved to another meeting, indicators that it was solved</t>
   </si>
   <si>
@@ -277,6 +268,15 @@
   </si>
   <si>
     <t>Permissions for VTO</t>
+  </si>
+  <si>
+    <t>Charts on Scorecard</t>
+  </si>
+  <si>
+    <t>https://mail.google.com/mail/u/0/#inbox/159d1194f9ac84ff</t>
+  </si>
+  <si>
+    <t>Mask Notes Url for editing</t>
   </si>
 </sst>
 </file>
@@ -665,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B1:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,67 +683,67 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="11">
-        <f>1-COUNTBLANK($A$6:A73)/ROWS($A$6:A73)</f>
-        <v>0.32352941176470584</v>
+        <f>1-COUNTBLANK($A$6:A70)/ROWS($A$6:A70)</f>
+        <v>0.56923076923076921</v>
       </c>
       <c r="I1" s="12">
         <f>H2/H3</f>
-        <v>0.3235294117647059</v>
+        <v>0.56923076923076921</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3">
-        <f>ROWS($A$6:A73)-COUNTBLANK($A$6:A73)</f>
-        <v>22</v>
+        <f>ROWS($A$6:A70)-COUNTBLANK($A$6:A70)</f>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="4">
-        <f>ROWS(A6:A73)</f>
-        <v>68</v>
+        <f>ROWS(A6:A70)</f>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="2">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C6" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="8">
         <f>SQRT(B6)*(C6)*IF(ISBLANK(A6),1,-1)</f>
-        <v>72</v>
+        <v>68.227560413662744</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6"/>
       <c r="H6" s="6"/>
@@ -751,17 +751,17 @@
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="2">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" s="8">
         <f>SQRT(B7)*(C7)*IF(ISBLANK(A7),1,-1)</f>
-        <v>68.227560413662744</v>
+        <v>63.63961030678928</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="F7"/>
       <c r="H7" s="6"/>
@@ -772,14 +772,14 @@
         <v>70</v>
       </c>
       <c r="C8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="8">
         <f>SQRT(B8)*(C8)*IF(ISBLANK(A8),1,-1)</f>
-        <v>66.932802122726045</v>
+        <v>58.566201857385288</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="F8"/>
       <c r="H8" s="6"/>
@@ -787,88 +787,86 @@
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D9" s="8">
         <f>SQRT(B9)*(C9)*IF(ISBLANK(A9),1,-1)</f>
-        <v>63.63961030678928</v>
+        <v>44.721359549995796</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F9"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10"/>
       <c r="B10" s="2">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C10" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" s="8">
         <f>SQRT(B10)*(C10)*IF(ISBLANK(A10),1,-1)</f>
-        <v>62.217360921209121</v>
-      </c>
-      <c r="E10" t="s">
-        <v>73</v>
+        <v>43.301270189221938</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11"/>
       <c r="B11" s="2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="8">
         <f>SQRT(B11)*(C11)*IF(ISBLANK(A11),1,-1)</f>
-        <v>58.566201857385288</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
+        <v>42.426406871192853</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="2"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12"/>
       <c r="B12" s="2">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="8">
         <f>SQRT(B12)*(C12)*IF(ISBLANK(A12),1,-1)</f>
-        <v>53.310411741047361</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>4</v>
+        <v>42.426406871192853</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="F12"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13"/>
       <c r="B13" s="2">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="8">
         <f>SQRT(B13)*(C13)*IF(ISBLANK(A13),1,-1)</f>
-        <v>50</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>40.693979898751607</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
       </c>
       <c r="F13"/>
       <c r="H13" s="6"/>
@@ -876,17 +874,17 @@
     <row r="14" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14" s="2">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2">
         <v>5</v>
       </c>
       <c r="D14" s="8">
         <f>SQRT(B14)*(C14)*IF(ISBLANK(A14),1,-1)</f>
-        <v>44.721359549995796</v>
+        <v>40.311288741492746</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="F14"/>
       <c r="H14" s="6"/>
@@ -894,86 +892,91 @@
     <row r="15" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15" s="2">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2">
         <v>5</v>
       </c>
       <c r="D15" s="8">
         <f>SQRT(B15)*(C15)*IF(ISBLANK(A15),1,-1)</f>
-        <v>44.158804331639239</v>
+        <v>40.311288741492746</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F15"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16"/>
       <c r="B16" s="2">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D16" s="8">
         <f>SQRT(B16)*(C16)*IF(ISBLANK(A16),1,-1)</f>
-        <v>43.301270189221938</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>64</v>
+        <v>38.340579025361627</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
       </c>
       <c r="F16"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17"/>
       <c r="B17" s="2">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="8">
         <f>SQRT(B17)*(C17)*IF(ISBLANK(A17),1,-1)</f>
-        <v>42.426406871192853</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>37.080992435478315</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
       </c>
       <c r="F17" s="2"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
       <c r="B18" s="2">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18" s="8">
         <f>SQRT(B18)*(C18)*IF(ISBLANK(A18),1,-1)</f>
-        <v>42.426406871192853</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>35.552777669262355</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
       </c>
       <c r="F18"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
+      <c r="A19" s="5">
+        <v>42762</v>
+      </c>
       <c r="B19" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" s="8">
         <f>SQRT(B19)*(C19)*IF(ISBLANK(A19),1,-1)</f>
-        <v>40.693979898751607</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
+        <v>-33.541019662496851</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="F19"/>
       <c r="H19" s="6"/>
@@ -981,17 +984,17 @@
     <row r="20" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20" s="2">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="8">
         <f>SQRT(B20)*(C20)*IF(ISBLANK(A20),1,-1)</f>
-        <v>40.311288741492746</v>
+        <v>30.724582991474431</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="F20" s="2"/>
       <c r="H20" s="6"/>
@@ -999,655 +1002,716 @@
     <row r="21" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21" s="2">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="8">
         <f>SQRT(B21)*(C21)*IF(ISBLANK(A21),1,-1)</f>
-        <v>40.311288741492746</v>
+        <v>30.724582991474431</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F21"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>42762</v>
+      </c>
       <c r="B22" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" s="8">
         <f>SQRT(B22)*(C22)*IF(ISBLANK(A22),1,-1)</f>
-        <v>38.340579025361627</v>
+        <v>-30</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
       <c r="B23" s="2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23" s="8">
         <f>SQRT(B23)*(C23)*IF(ISBLANK(A23),1,-1)</f>
-        <v>37.947331922020552</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>66</v>
+        <v>26.832815729997478</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="8">
         <f>SQRT(B24)*(C24)*IF(ISBLANK(A24),1,-1)</f>
-        <v>37.080992435478315</v>
+        <v>26.832815729997478</v>
       </c>
       <c r="E24" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
       <c r="B25" s="2">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="8">
         <f>SQRT(B25)*(C25)*IF(ISBLANK(A25),1,-1)</f>
-        <v>35.552777669262355</v>
-      </c>
-      <c r="E25" t="s">
-        <v>7</v>
+        <v>24.919871588754226</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D26" s="8">
         <f>SQRT(B26)*(C26)*IF(ISBLANK(A26),1,-1)</f>
-        <v>33.541019662496851</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>0</v>
+        <v>24.556058315617349</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2">
         <v>3</v>
       </c>
       <c r="D27" s="8">
         <f>SQRT(B27)*(C27)*IF(ISBLANK(A27),1,-1)</f>
-        <v>30.740852297878796</v>
+        <v>24.186773244895647</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="8">
         <f>SQRT(B28)*(C28)*IF(ISBLANK(A28),1,-1)</f>
-        <v>30.724582991474431</v>
-      </c>
-      <c r="E28" t="s">
-        <v>56</v>
+        <v>23.237900077244504</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C29" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="8">
         <f>SQRT(B29)*(C29)*IF(ISBLANK(A29),1,-1)</f>
-        <v>30.724582991474431</v>
+        <v>17.748239349298849</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C30" s="2">
         <v>3</v>
       </c>
       <c r="D30" s="8">
         <f>SQRT(B30)*(C30)*IF(ISBLANK(A30),1,-1)</f>
-        <v>30.14962686336267</v>
+        <v>16.431676725154983</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2">
-        <v>100</v>
-      </c>
-      <c r="C31" s="2">
-        <v>3</v>
+      <c r="B31">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
       </c>
       <c r="D31" s="8">
         <f>SQRT(B31)*(C31)*IF(ISBLANK(A31),1,-1)</f>
-        <v>30</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>74</v>
+        <v>12.649110640673518</v>
+      </c>
+      <c r="E31" t="s">
+        <v>58</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>25</v>
-      </c>
-      <c r="C32" s="2">
-        <v>6</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
       <c r="D32" s="8">
         <f>SQRT(B32)*(C32)*IF(ISBLANK(A32),1,-1)</f>
-        <v>30</v>
-      </c>
-      <c r="E32" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
-        <v>45</v>
-      </c>
-      <c r="C33" s="2">
-        <v>4</v>
-      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
       <c r="D33" s="8">
         <f>SQRT(B33)*(C33)*IF(ISBLANK(A33),1,-1)</f>
-        <v>26.832815729997478</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
-        <v>45</v>
-      </c>
-      <c r="C34" s="2">
-        <v>4</v>
-      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
       <c r="D34" s="8">
         <f>SQRT(B34)*(C34)*IF(ISBLANK(A34),1,-1)</f>
-        <v>26.832815729997478</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2">
-        <v>75</v>
-      </c>
-      <c r="C35" s="2">
-        <v>3</v>
-      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
       <c r="D35" s="8">
         <f>SQRT(B35)*(C35)*IF(ISBLANK(A35),1,-1)</f>
-        <v>25.98076211353316</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="5">
+        <v>42736</v>
+      </c>
       <c r="B36" s="2">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D36" s="8">
         <f>SQRT(B36)*(C36)*IF(ISBLANK(A36),1,-1)</f>
-        <v>24.919871588754226</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>40</v>
+        <v>-1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>42701</v>
+      </c>
       <c r="B37" s="2">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="C37" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D37" s="8">
         <f>SQRT(B37)*(C37)*IF(ISBLANK(A37),1,-1)</f>
-        <v>24.556058315617349</v>
-      </c>
-      <c r="E37" t="s">
-        <v>59</v>
+        <v>-1</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>42701</v>
+      </c>
       <c r="B38" s="2">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="C38" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D38" s="8">
         <f>SQRT(B38)*(C38)*IF(ISBLANK(A38),1,-1)</f>
-        <v>24.186773244895647</v>
-      </c>
-      <c r="E38" t="s">
-        <v>52</v>
+        <v>-1</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>42697</v>
+      </c>
       <c r="B39" s="2">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C39" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D39" s="8">
         <f>SQRT(B39)*(C39)*IF(ISBLANK(A39),1,-1)</f>
-        <v>23.237900077244504</v>
+        <v>-1</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>42696</v>
+      </c>
       <c r="B40" s="2">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" s="8">
         <f>SQRT(B40)*(C40)*IF(ISBLANK(A40),1,-1)</f>
-        <v>17.748239349298849</v>
+        <v>-1</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="9">
+        <v>42681</v>
+      </c>
       <c r="B41" s="2">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C41" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D41" s="8">
         <f>SQRT(B41)*(C41)*IF(ISBLANK(A41),1,-1)</f>
-        <v>16.431676725154983</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F41" s="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>40</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
+      <c r="A42" s="9">
+        <v>42696</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
       </c>
       <c r="D42" s="8">
         <f>SQRT(B42)*(C42)*IF(ISBLANK(A42),1,-1)</f>
-        <v>12.649110640673518</v>
+        <v>-1</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="9">
+        <v>42688</v>
+      </c>
       <c r="B43" s="2">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C43" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="8">
         <f>SQRT(B43)*(C43)*IF(ISBLANK(A43),1,-1)</f>
-        <v>10</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>39</v>
+        <v>-1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B44" s="2">
+        <v>25</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2</v>
+      </c>
       <c r="D44" s="8">
         <f>SQRT(B44)*(C44)*IF(ISBLANK(A44),1,-1)</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="10">
+        <v>42706</v>
+      </c>
+      <c r="B45" s="2">
+        <v>60</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2</v>
+      </c>
       <c r="D45" s="8">
         <f>SQRT(B45)*(C45)*IF(ISBLANK(A45),1,-1)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>16</v>
-      </c>
+        <v>-15.491933384829668</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="5">
+        <v>42706</v>
+      </c>
+      <c r="B46" s="2">
+        <v>75</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2</v>
+      </c>
       <c r="D46" s="8">
         <f>SQRT(B46)*(C46)*IF(ISBLANK(A46),1,-1)</f>
-        <v>0</v>
+        <v>-17.320508075688775</v>
       </c>
       <c r="E46" t="s">
-        <v>17</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="A47" s="10">
+        <v>42742</v>
+      </c>
+      <c r="B47" s="2">
+        <v>75</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3</v>
+      </c>
       <c r="D47" s="8">
         <f>SQRT(B47)*(C47)*IF(ISBLANK(A47),1,-1)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" t="s">
-        <v>18</v>
-      </c>
+        <v>-25.98076211353316</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="A48" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B48" s="2">
+        <v>100</v>
+      </c>
+      <c r="C48" s="2">
+        <v>3</v>
+      </c>
       <c r="D48" s="8">
         <f>SQRT(B48)*(C48)*IF(ISBLANK(A48),1,-1)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>23</v>
+        <v>-30</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="A49" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B49" s="2">
+        <v>101</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3</v>
+      </c>
       <c r="D49" s="8">
         <f>SQRT(B49)*(C49)*IF(ISBLANK(A49),1,-1)</f>
-        <v>0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="2"/>
+        <v>-30.14962686336267</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="5">
+        <v>42736</v>
+      </c>
+      <c r="B50" s="2">
+        <v>105</v>
+      </c>
+      <c r="C50" s="2">
+        <v>3</v>
+      </c>
       <c r="D50" s="8">
         <f>SQRT(B50)*(C50)*IF(ISBLANK(A50),1,-1)</f>
-        <v>0</v>
+        <v>-30.740852297878796</v>
       </c>
       <c r="E50" t="s">
-        <v>58</v>
-      </c>
-      <c r="F50" s="2"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="A51" s="10">
+        <v>42709</v>
+      </c>
+      <c r="B51" s="2">
+        <v>50</v>
+      </c>
+      <c r="C51" s="2">
+        <v>5</v>
+      </c>
       <c r="D51" s="8">
         <f>SQRT(B51)*(C51)*IF(ISBLANK(A51),1,-1)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51" s="2"/>
+        <v>-35.355339059327378</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
-        <v>42701</v>
+      <c r="A52" s="10">
+        <v>42758</v>
       </c>
       <c r="B52" s="2">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C52" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D52" s="8">
         <f>SQRT(B52)*(C52)*IF(ISBLANK(A52),1,-1)</f>
-        <v>-1</v>
+        <v>-37.947331922020552</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
-        <v>42701</v>
+      <c r="A53" s="5">
+        <v>42706</v>
       </c>
       <c r="B53" s="2">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C53" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D53" s="8">
         <f>SQRT(B53)*(C53)*IF(ISBLANK(A53),1,-1)</f>
-        <v>-1</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>-42.720018726587654</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
-        <v>42697</v>
+      <c r="A54" s="5">
+        <v>42736</v>
       </c>
       <c r="B54" s="2">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="C54" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D54" s="8">
         <f>SQRT(B54)*(C54)*IF(ISBLANK(A54),1,-1)</f>
-        <v>-1</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>41</v>
+        <v>-44.158804331639239</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
-        <v>42696</v>
+      <c r="A55" s="10">
+        <v>42706</v>
       </c>
       <c r="B55" s="2">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D55" s="8">
         <f>SQRT(B55)*(C55)*IF(ISBLANK(A55),1,-1)</f>
-        <v>-1</v>
-      </c>
-      <c r="E55" t="s">
-        <v>8</v>
+        <v>-44.497190922573978</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
-        <v>42681</v>
+      <c r="A56" s="10">
+        <v>42742</v>
       </c>
       <c r="B56" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C56" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D56" s="8">
         <f>SQRT(B56)*(C56)*IF(ISBLANK(A56),1,-1)</f>
-        <v>-1</v>
-      </c>
-      <c r="E56" t="s">
-        <v>14</v>
-      </c>
-      <c r="F56" s="2"/>
+        <v>-50</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
-        <v>42696</v>
+      <c r="A57" s="5">
+        <v>42744</v>
       </c>
       <c r="B57" s="2">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C57" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D57" s="8">
         <f>SQRT(B57)*(C57)*IF(ISBLANK(A57),1,-1)</f>
-        <v>-1</v>
-      </c>
-      <c r="E57" t="s">
-        <v>25</v>
+        <v>-53.310411741047361</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
-        <v>42688</v>
+      <c r="A58" s="10">
+        <v>42706</v>
       </c>
       <c r="B58" s="2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C58" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D58" s="8">
         <f>SQRT(B58)*(C58)*IF(ISBLANK(A58),1,-1)</f>
-        <v>-1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>27</v>
+        <v>-54.772255750516614</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="10">
-        <v>42706</v>
+      <c r="A59" s="5">
+        <v>42709</v>
       </c>
       <c r="B59" s="2">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C59" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D59" s="8">
         <f>SQRT(B59)*(C59)*IF(ISBLANK(A59),1,-1)</f>
-        <v>-15.491933384829668</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>37</v>
+        <v>-60</v>
+      </c>
+      <c r="E59" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>42706</v>
+        <v>42749</v>
       </c>
       <c r="B60" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C60" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D60" s="8">
         <f>SQRT(B60)*(C60)*IF(ISBLANK(A60),1,-1)</f>
-        <v>-17.320508075688775</v>
+        <v>-62.217360921209121</v>
       </c>
       <c r="E60" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="10">
-        <v>42709</v>
+      <c r="A61" s="5">
+        <v>42705</v>
       </c>
       <c r="B61" s="2">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C61" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D61" s="8">
         <f>SQRT(B61)*(C61)*IF(ISBLANK(A61),1,-1)</f>
-        <v>-35.355339059327378</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>68</v>
+        <v>-66.775744099186198</v>
+      </c>
+      <c r="E61" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <v>42706</v>
+        <v>42754</v>
       </c>
       <c r="B62" s="2">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C62" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D62" s="8">
         <f>SQRT(B62)*(C62)*IF(ISBLANK(A62),1,-1)</f>
-        <v>-42.720018726587654</v>
+        <v>-66.932802122726045</v>
       </c>
       <c r="E62" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1655,53 +1719,53 @@
         <v>42706</v>
       </c>
       <c r="B63" s="2">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C63" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D63" s="8">
         <f>SQRT(B63)*(C63)*IF(ISBLANK(A63),1,-1)</f>
-        <v>-44.497190922573978</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>38</v>
+        <v>-66.932802122726045</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
-        <v>42706</v>
+        <v>42705</v>
       </c>
       <c r="B64" s="2">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="C64" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D64" s="8">
         <f>SQRT(B64)*(C64)*IF(ISBLANK(A64),1,-1)</f>
-        <v>-54.772255750516614</v>
-      </c>
-      <c r="E64" s="2" t="s">
+        <v>-70.710678118654755</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
-        <v>42709</v>
+      <c r="A65" s="9">
+        <v>42705</v>
       </c>
       <c r="B65" s="2">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C65" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D65" s="8">
         <f>SQRT(B65)*(C65)*IF(ISBLANK(A65),1,-1)</f>
-        <v>-60</v>
-      </c>
-      <c r="E65" t="s">
-        <v>72</v>
+        <v>-71.105555338524709</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,148 +1773,94 @@
         <v>42705</v>
       </c>
       <c r="B66" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C66" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D66" s="8">
         <f>SQRT(B66)*(C66)*IF(ISBLANK(A66),1,-1)</f>
-        <v>-66.775744099186198</v>
-      </c>
-      <c r="E66" t="s">
-        <v>22</v>
+        <v>-71.554175279993274</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="10">
-        <v>42706</v>
+      <c r="A67" s="5">
+        <v>42754</v>
       </c>
       <c r="B67" s="2">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C67" s="2">
         <v>8</v>
       </c>
       <c r="D67" s="8">
         <f>SQRT(B67)*(C67)*IF(ISBLANK(A67),1,-1)</f>
-        <v>-66.932802122726045</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>35</v>
+        <v>-72</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="10">
-        <v>42705</v>
+      <c r="A68" s="5">
+        <v>42706</v>
       </c>
       <c r="B68" s="2">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="C68" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D68" s="8">
         <f>SQRT(B68)*(C68)*IF(ISBLANK(A68),1,-1)</f>
-        <v>-70.710678118654755</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>70</v>
+        <v>-73.416619371910613</v>
+      </c>
+      <c r="E68" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
-        <v>42705</v>
+      <c r="A69" s="5">
+        <v>42701</v>
       </c>
       <c r="B69" s="2">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C69" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D69" s="8">
         <f>SQRT(B69)*(C69)*IF(ISBLANK(A69),1,-1)</f>
-        <v>-71.105555338524709</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>31</v>
+        <v>-89.095454429504983</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
-        <v>42705</v>
+      <c r="A70" s="9">
+        <v>42703</v>
       </c>
       <c r="B70" s="2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C70" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D70" s="8">
         <f>SQRT(B70)*(C70)*IF(ISBLANK(A70),1,-1)</f>
-        <v>-71.554175279993274</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <v>42706</v>
-      </c>
-      <c r="B71" s="2">
-        <v>110</v>
-      </c>
-      <c r="C71" s="2">
-        <v>7</v>
-      </c>
-      <c r="D71" s="8">
-        <f>SQRT(B71)*(C71)*IF(ISBLANK(A71),1,-1)</f>
-        <v>-73.416619371910613</v>
-      </c>
-      <c r="E71" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
-        <v>42701</v>
-      </c>
-      <c r="B72" s="2">
-        <v>98</v>
-      </c>
-      <c r="C72" s="2">
-        <v>9</v>
-      </c>
-      <c r="D72" s="8">
-        <f>SQRT(B72)*(C72)*IF(ISBLANK(A72),1,-1)</f>
-        <v>-89.095454429504983</v>
-      </c>
-      <c r="E72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
-        <v>42703</v>
-      </c>
-      <c r="B73" s="2">
-        <v>100</v>
-      </c>
-      <c r="C73" s="2">
-        <v>10</v>
-      </c>
-      <c r="D73" s="8">
-        <f>SQRT(B73)*(C73)*IF(ISBLANK(A73),1,-1)</f>
         <v>-100</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>63</v>
+      <c r="E70" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A5:E5">
-    <sortState ref="A6:E73">
+    <sortState ref="A6:E70">
       <sortCondition descending="1" ref="D5"/>
     </sortState>
   </autoFilter>
@@ -1876,46 +1886,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A2:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
VS nulled all my files >:(
</commit_message>
<xml_diff>
--- a/20161127 todos.xlsx
+++ b/20161127 todos.xlsx
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Current!$A$5:$E$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -668,7 +669,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,11 +688,11 @@
       </c>
       <c r="H1" s="11">
         <f>1-COUNTBLANK($A$6:A70)/ROWS($A$6:A70)</f>
-        <v>0.56923076923076921</v>
+        <v>0.72307692307692306</v>
       </c>
       <c r="I1" s="12">
         <f>H2/H3</f>
-        <v>0.56923076923076921</v>
+        <v>0.72307692307692306</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -700,7 +701,7 @@
       </c>
       <c r="H2" s="3">
         <f>ROWS($A$6:A70)-COUNTBLANK($A$6:A70)</f>
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -739,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="8">
-        <f>SQRT(B6)*(C6)*IF(ISBLANK(A6),1,-1)</f>
+        <f t="shared" ref="D6:D37" si="0">SQRT(B6)*(C6)*IF(ISBLANK(A6),1,-1)</f>
         <v>68.227560413662744</v>
       </c>
       <c r="E6" t="s">
@@ -749,7 +750,9 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7"/>
+      <c r="A7">
+        <v>1</v>
+      </c>
       <c r="B7" s="2">
         <v>50</v>
       </c>
@@ -757,8 +760,8 @@
         <v>9</v>
       </c>
       <c r="D7" s="8">
-        <f>SQRT(B7)*(C7)*IF(ISBLANK(A7),1,-1)</f>
-        <v>63.63961030678928</v>
+        <f t="shared" si="0"/>
+        <v>-63.63961030678928</v>
       </c>
       <c r="E7" t="s">
         <v>68</v>
@@ -775,7 +778,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="8">
-        <f>SQRT(B8)*(C8)*IF(ISBLANK(A8),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>58.566201857385288</v>
       </c>
       <c r="E8" t="s">
@@ -793,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="8">
-        <f>SQRT(B9)*(C9)*IF(ISBLANK(A9),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>44.721359549995796</v>
       </c>
       <c r="E9" t="s">
@@ -810,7 +813,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="8">
-        <f>SQRT(B10)*(C10)*IF(ISBLANK(A10),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>43.301270189221938</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -827,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="8">
-        <f>SQRT(B11)*(C11)*IF(ISBLANK(A11),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>42.426406871192853</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -837,6 +840,9 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
       <c r="B12" s="2">
         <v>50</v>
       </c>
@@ -844,8 +850,8 @@
         <v>6</v>
       </c>
       <c r="D12" s="8">
-        <f>SQRT(B12)*(C12)*IF(ISBLANK(A12),1,-1)</f>
-        <v>42.426406871192853</v>
+        <f t="shared" si="0"/>
+        <v>-42.426406871192853</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>35</v>
@@ -862,7 +868,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="8">
-        <f>SQRT(B13)*(C13)*IF(ISBLANK(A13),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>40.693979898751607</v>
       </c>
       <c r="E13" t="s">
@@ -880,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="8">
-        <f>SQRT(B14)*(C14)*IF(ISBLANK(A14),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>40.311288741492746</v>
       </c>
       <c r="E14" t="s">
@@ -898,7 +904,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="8">
-        <f>SQRT(B15)*(C15)*IF(ISBLANK(A15),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>40.311288741492746</v>
       </c>
       <c r="E15" t="s">
@@ -916,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="8">
-        <f>SQRT(B16)*(C16)*IF(ISBLANK(A16),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>38.340579025361627</v>
       </c>
       <c r="E16" t="s">
@@ -926,7 +932,9 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
+      <c r="A17">
+        <v>1</v>
+      </c>
       <c r="B17" s="2">
         <v>55</v>
       </c>
@@ -934,8 +942,8 @@
         <v>5</v>
       </c>
       <c r="D17" s="8">
-        <f>SQRT(B17)*(C17)*IF(ISBLANK(A17),1,-1)</f>
-        <v>37.080992435478315</v>
+        <f t="shared" si="0"/>
+        <v>-37.080992435478315</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -952,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="8">
-        <f>SQRT(B18)*(C18)*IF(ISBLANK(A18),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>35.552777669262355</v>
       </c>
       <c r="E18" t="s">
@@ -972,7 +980,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="8">
-        <f>SQRT(B19)*(C19)*IF(ISBLANK(A19),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>-33.541019662496851</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -982,7 +990,9 @@
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
+      <c r="A20">
+        <v>1</v>
+      </c>
       <c r="B20" s="2">
         <v>59</v>
       </c>
@@ -990,8 +1000,8 @@
         <v>4</v>
       </c>
       <c r="D20" s="8">
-        <f>SQRT(B20)*(C20)*IF(ISBLANK(A20),1,-1)</f>
-        <v>30.724582991474431</v>
+        <f t="shared" si="0"/>
+        <v>-30.724582991474431</v>
       </c>
       <c r="E20" t="s">
         <v>54</v>
@@ -1000,7 +1010,9 @@
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
+      <c r="A21">
+        <v>1</v>
+      </c>
       <c r="B21" s="2">
         <v>59</v>
       </c>
@@ -1008,8 +1020,8 @@
         <v>4</v>
       </c>
       <c r="D21" s="8">
-        <f>SQRT(B21)*(C21)*IF(ISBLANK(A21),1,-1)</f>
-        <v>30.724582991474431</v>
+        <f t="shared" si="0"/>
+        <v>-30.724582991474431</v>
       </c>
       <c r="E21" t="s">
         <v>55</v>
@@ -1028,7 +1040,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="8">
-        <f>SQRT(B22)*(C22)*IF(ISBLANK(A22),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>-30</v>
       </c>
       <c r="E22" t="s">
@@ -1043,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="8">
-        <f>SQRT(B23)*(C23)*IF(ISBLANK(A23),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>26.832815729997478</v>
       </c>
       <c r="E23" t="s">
@@ -1059,7 +1071,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="8">
-        <f>SQRT(B24)*(C24)*IF(ISBLANK(A24),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>26.832815729997478</v>
       </c>
       <c r="E24" t="s">
@@ -1075,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="8">
-        <f>SQRT(B25)*(C25)*IF(ISBLANK(A25),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>24.919871588754226</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -1083,6 +1095,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
       <c r="B26" s="2">
         <v>67</v>
       </c>
@@ -1090,8 +1105,8 @@
         <v>3</v>
       </c>
       <c r="D26" s="8">
-        <f>SQRT(B26)*(C26)*IF(ISBLANK(A26),1,-1)</f>
-        <v>24.556058315617349</v>
+        <f t="shared" si="0"/>
+        <v>-24.556058315617349</v>
       </c>
       <c r="E26" t="s">
         <v>56</v>
@@ -1106,7 +1121,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="8">
-        <f>SQRT(B27)*(C27)*IF(ISBLANK(A27),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>24.186773244895647</v>
       </c>
       <c r="E27" t="s">
@@ -1114,6 +1129,9 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
       <c r="B28" s="2">
         <v>60</v>
       </c>
@@ -1121,8 +1139,8 @@
         <v>3</v>
       </c>
       <c r="D28" s="8">
-        <f>SQRT(B28)*(C28)*IF(ISBLANK(A28),1,-1)</f>
-        <v>23.237900077244504</v>
+        <f t="shared" si="0"/>
+        <v>-23.237900077244504</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>50</v>
@@ -1136,7 +1154,7 @@
         <v>3</v>
       </c>
       <c r="D29" s="8">
-        <f>SQRT(B29)*(C29)*IF(ISBLANK(A29),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>17.748239349298849</v>
       </c>
       <c r="E29" t="s">
@@ -1152,7 +1170,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="8">
-        <f>SQRT(B30)*(C30)*IF(ISBLANK(A30),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>16.431676725154983</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -1167,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="8">
-        <f>SQRT(B31)*(C31)*IF(ISBLANK(A31),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>12.649110640673518</v>
       </c>
       <c r="E31" t="s">
@@ -1179,7 +1197,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="8">
-        <f>SQRT(B32)*(C32)*IF(ISBLANK(A32),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -1188,10 +1206,13 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-1</v>
+      </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="8">
-        <f>SQRT(B33)*(C33)*IF(ISBLANK(A33),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E33" t="s">
@@ -1199,10 +1220,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-1</v>
+      </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="8">
-        <f>SQRT(B34)*(C34)*IF(ISBLANK(A34),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E34" t="s">
@@ -1210,10 +1234,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-1</v>
+      </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="8">
-        <f>SQRT(B35)*(C35)*IF(ISBLANK(A35),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E35" t="s">
@@ -1231,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="8">
-        <f>SQRT(B36)*(C36)*IF(ISBLANK(A36),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="E36" t="s">
@@ -1250,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="8">
-        <f>SQRT(B37)*(C37)*IF(ISBLANK(A37),1,-1)</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -1268,7 +1295,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="8">
-        <f>SQRT(B38)*(C38)*IF(ISBLANK(A38),1,-1)</f>
+        <f t="shared" ref="D38:D69" si="1">SQRT(B38)*(C38)*IF(ISBLANK(A38),1,-1)</f>
         <v>-1</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -1287,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="8">
-        <f>SQRT(B39)*(C39)*IF(ISBLANK(A39),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -1306,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="8">
-        <f>SQRT(B40)*(C40)*IF(ISBLANK(A40),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="E40" t="s">
@@ -1324,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="8">
-        <f>SQRT(B41)*(C41)*IF(ISBLANK(A41),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="E41" t="s">
@@ -1342,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="8">
-        <f>SQRT(B42)*(C42)*IF(ISBLANK(A42),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="E42" t="s">
@@ -1360,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="8">
-        <f>SQRT(B43)*(C43)*IF(ISBLANK(A43),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="E43" t="s">
@@ -1378,7 +1405,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="8">
-        <f>SQRT(B44)*(C44)*IF(ISBLANK(A44),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-10</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -1396,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="8">
-        <f>SQRT(B45)*(C45)*IF(ISBLANK(A45),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-15.491933384829668</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -1415,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="8">
-        <f>SQRT(B46)*(C46)*IF(ISBLANK(A46),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-17.320508075688775</v>
       </c>
       <c r="E46" t="s">
@@ -1434,7 +1461,7 @@
         <v>3</v>
       </c>
       <c r="D47" s="8">
-        <f>SQRT(B47)*(C47)*IF(ISBLANK(A47),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-25.98076211353316</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -1453,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="D48" s="8">
-        <f>SQRT(B48)*(C48)*IF(ISBLANK(A48),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-30</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -1472,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="D49" s="8">
-        <f>SQRT(B49)*(C49)*IF(ISBLANK(A49),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-30.14962686336267</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -1490,7 +1517,7 @@
         <v>3</v>
       </c>
       <c r="D50" s="8">
-        <f>SQRT(B50)*(C50)*IF(ISBLANK(A50),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-30.740852297878796</v>
       </c>
       <c r="E50" t="s">
@@ -1508,7 +1535,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="8">
-        <f>SQRT(B51)*(C51)*IF(ISBLANK(A51),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-35.355339059327378</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -1526,7 +1553,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="8">
-        <f>SQRT(B52)*(C52)*IF(ISBLANK(A52),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-37.947331922020552</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -1544,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="D53" s="8">
-        <f>SQRT(B53)*(C53)*IF(ISBLANK(A53),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-42.720018726587654</v>
       </c>
       <c r="E53" t="s">
@@ -1563,7 +1590,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="8">
-        <f>SQRT(B54)*(C54)*IF(ISBLANK(A54),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-44.158804331639239</v>
       </c>
       <c r="E54" t="s">
@@ -1581,7 +1608,7 @@
         <v>6</v>
       </c>
       <c r="D55" s="8">
-        <f>SQRT(B55)*(C55)*IF(ISBLANK(A55),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-44.497190922573978</v>
       </c>
       <c r="E55" s="14" t="s">
@@ -1599,7 +1626,7 @@
         <v>5</v>
       </c>
       <c r="D56" s="8">
-        <f>SQRT(B56)*(C56)*IF(ISBLANK(A56),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-50</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -1617,7 +1644,7 @@
         <v>7</v>
       </c>
       <c r="D57" s="8">
-        <f>SQRT(B57)*(C57)*IF(ISBLANK(A57),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-53.310411741047361</v>
       </c>
       <c r="E57" s="13" t="s">
@@ -1635,7 +1662,7 @@
         <v>10</v>
       </c>
       <c r="D58" s="8">
-        <f>SQRT(B58)*(C58)*IF(ISBLANK(A58),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-54.772255750516614</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -1653,7 +1680,7 @@
         <v>6</v>
       </c>
       <c r="D59" s="8">
-        <f>SQRT(B59)*(C59)*IF(ISBLANK(A59),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-60</v>
       </c>
       <c r="E59" t="s">
@@ -1671,7 +1698,7 @@
         <v>7</v>
       </c>
       <c r="D60" s="8">
-        <f>SQRT(B60)*(C60)*IF(ISBLANK(A60),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-62.217360921209121</v>
       </c>
       <c r="E60" t="s">
@@ -1689,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="D61" s="8">
-        <f>SQRT(B61)*(C61)*IF(ISBLANK(A61),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-66.775744099186198</v>
       </c>
       <c r="E61" t="s">
@@ -1707,7 +1734,7 @@
         <v>8</v>
       </c>
       <c r="D62" s="8">
-        <f>SQRT(B62)*(C62)*IF(ISBLANK(A62),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-66.932802122726045</v>
       </c>
       <c r="E62" t="s">
@@ -1725,7 +1752,7 @@
         <v>8</v>
       </c>
       <c r="D63" s="8">
-        <f>SQRT(B63)*(C63)*IF(ISBLANK(A63),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-66.932802122726045</v>
       </c>
       <c r="E63" s="2" t="s">
@@ -1743,7 +1770,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="8">
-        <f>SQRT(B64)*(C64)*IF(ISBLANK(A64),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-70.710678118654755</v>
       </c>
       <c r="E64" s="1" t="s">
@@ -1761,7 +1788,7 @@
         <v>8</v>
       </c>
       <c r="D65" s="8">
-        <f>SQRT(B65)*(C65)*IF(ISBLANK(A65),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-71.105555338524709</v>
       </c>
       <c r="E65" s="1" t="s">
@@ -1779,7 +1806,7 @@
         <v>8</v>
       </c>
       <c r="D66" s="8">
-        <f>SQRT(B66)*(C66)*IF(ISBLANK(A66),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-71.554175279993274</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -1797,7 +1824,7 @@
         <v>8</v>
       </c>
       <c r="D67" s="8">
-        <f>SQRT(B67)*(C67)*IF(ISBLANK(A67),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-72</v>
       </c>
       <c r="E67" t="s">
@@ -1815,7 +1842,7 @@
         <v>7</v>
       </c>
       <c r="D68" s="8">
-        <f>SQRT(B68)*(C68)*IF(ISBLANK(A68),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-73.416619371910613</v>
       </c>
       <c r="E68" t="s">
@@ -1833,7 +1860,7 @@
         <v>9</v>
       </c>
       <c r="D69" s="8">
-        <f>SQRT(B69)*(C69)*IF(ISBLANK(A69),1,-1)</f>
+        <f t="shared" si="1"/>
         <v>-89.095454429504983</v>
       </c>
       <c r="E69" t="s">
@@ -1851,7 +1878,7 @@
         <v>10</v>
       </c>
       <c r="D70" s="8">
-        <f>SQRT(B70)*(C70)*IF(ISBLANK(A70),1,-1)</f>
+        <f t="shared" ref="D70:D101" si="2">SQRT(B70)*(C70)*IF(ISBLANK(A70),1,-1)</f>
         <v>-100</v>
       </c>
       <c r="E70" s="2" t="s">

</xml_diff>